<commit_message>
1. auto fit columns width 2. just display specified columns
</commit_message>
<xml_diff>
--- a/AutomationExcelOperation/AutomationExcelOperation/Data/GeneratedExcel/Order.xlsx
+++ b/AutomationExcelOperation/AutomationExcelOperation/Data/GeneratedExcel/Order.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ProductId</t>
   </si>
@@ -36,31 +36,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Tokens</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
     <t>1234</t>
   </si>
   <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Mike</t>
   </si>
   <si>
     <t>3456</t>
-  </si>
-  <si>
-    <t>Chen</t>
   </si>
 </sst>
 </file>
@@ -116,14 +101,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E3">
-  <autoFilter ref="A1:E3"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D1:F3">
+  <autoFilter ref="D1:F3"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="UserId"/>
     <tableColumn id="2" name="UserName"/>
     <tableColumn id="3" name="Password"/>
-    <tableColumn id="4" name="Name"/>
-    <tableColumn id="5" name="Tokens"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -171,61 +154,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="D1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="9.39390999930245" customWidth="1"/>
+    <col min="5" max="5" width="12.9418999808175" customWidth="1"/>
+    <col min="6" max="6" width="12.0651332310268" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="0" t="s">
+    </row>
+    <row r="2">
+      <c r="D2" s="0">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="3">
+      <c r="D3" s="0">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some format fuction
</commit_message>
<xml_diff>
--- a/AutomationExcelOperation/AutomationExcelOperation/Data/GeneratedExcel/Order.xlsx
+++ b/AutomationExcelOperation/AutomationExcelOperation/Data/GeneratedExcel/Order.xlsx
@@ -6,7 +6,7 @@
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="User" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -53,10 +53,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000" tint="0"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -79,8 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,6 +131,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.2472392490932" customWidth="1"/>
+    <col min="2" max="2" width="15.7952292306083" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
@@ -154,47 +170,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="D1:F3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.39390999930245" customWidth="1"/>
-    <col min="5" max="5" width="12.9418999808175" customWidth="1"/>
-    <col min="6" max="6" width="12.0651332310268" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" style="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1" style="1"/>
+    <col min="4" max="4" width="9.39390999930245" customWidth="1" style="1"/>
+    <col min="5" max="5" width="12.9418999808175" customWidth="1" style="1"/>
+    <col min="6" max="16384" width="12.0651332310268" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="D2" s="0">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="0">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>